<commit_message>
Added new tags and beacon scanning feature
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Tags" sheetId="2" r:id="rId2"/>
+    <sheet name="Errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="142">
   <si>
     <t>Inputs</t>
   </si>
@@ -44,280 +45,403 @@
     <t>Tag URL</t>
   </si>
   <si>
+    <t>Google Tag Manager</t>
+  </si>
+  <si>
+    <t>https://www.googletagmanager.com/gtm.js?id=GTM-NM7FHHL</t>
+  </si>
+  <si>
+    <t>www.googletagmanager.com</t>
+  </si>
+  <si>
+    <t>OneTrust</t>
+  </si>
+  <si>
+    <t>https://geolocation.onetrust.com/cookieconsentpub/v1/geo/location</t>
+  </si>
+  <si>
+    <t>geolocation.onetrust.com</t>
+  </si>
+  <si>
+    <t>cdn.cookielaw.org</t>
+  </si>
+  <si>
+    <t>DoubleClick Floodlight</t>
+  </si>
+  <si>
+    <t>Google Global Site Tag (gtag.js)</t>
+  </si>
+  <si>
+    <t>youtube.com</t>
+  </si>
+  <si>
+    <t>where-to-buy.co</t>
+  </si>
+  <si>
+    <t>themes.googleusercontent.com</t>
+  </si>
+  <si>
+    <t>d22xmn10vbouk4.cloudfront.net</t>
+  </si>
+  <si>
+    <t>privacy.gsk.com</t>
+  </si>
+  <si>
+    <t>www.youtube.com</t>
+  </si>
+  <si>
+    <t>www.triaminic.com</t>
+  </si>
+  <si>
+    <t>www.theraflu.com</t>
+  </si>
+  <si>
+    <t>terms.gsk.com</t>
+  </si>
+  <si>
+    <t>cookies.gsk.com</t>
+  </si>
+  <si>
     <t>Google Universal Analytics</t>
   </si>
   <si>
+    <t>https://www.google-analytics.com/analytics.js</t>
+  </si>
+  <si>
+    <t>https://www.google-analytics.com/collect?v=1&amp;_v=j90&amp;a=1539169358&amp;t=pageview&amp;_s=1&amp;dl=https%3A%2F%2Fwww.abreva.ca%2F&amp;ul=en-us&amp;de=UTF-8&amp;dt=Works%20Faster*%20to%20Shorten%20Cold%20Sore%20Healing%20Time%20%7C%20Abreva&amp;sd=24-bit&amp;sr=1680x927&amp;vp=1680x927&amp;je=0&amp;_u=YGBAgEAB~&amp;jid=2124740992&amp;gjid=72677699&amp;cid=400124895.1619917863&amp;tid=UA-41812365-2&amp;_gid=1799241526.1619917863&amp;gtm=2wg4l3THX7RJS&amp;z=1791564017</t>
+  </si>
+  <si>
     <t>www.google-analytics.com</t>
   </si>
   <si>
-    <t>Google Tag Manager</t>
-  </si>
-  <si>
-    <t>www.googletagmanager.com</t>
-  </si>
-  <si>
-    <t>Google Global Site Tag (gtag.js)</t>
-  </si>
-  <si>
-    <t>privacy.gsk.com</t>
+    <t>https://www.googletagmanager.com/gtm.js?id=GTM-THX7RJS</t>
+  </si>
+  <si>
+    <t>Google Ads Audience Tracker</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>DoubleClick</t>
+  </si>
+  <si>
+    <t>https://stats.g.doubleclick.net/j/collect?t=dc&amp;aip=1&amp;_r=3&amp;v=1&amp;_v=j90&amp;tid=UA-41812365-2&amp;cid=400124895.1619917863&amp;jid=2124740992&amp;gjid=72677699&amp;_gid=1799241526.1619917863&amp;_u=YGBAgEABAAAAAE~&amp;z=248255208</t>
+  </si>
+  <si>
+    <t>stats.g.doubleclick.net</t>
+  </si>
+  <si>
+    <t>Google Web Font</t>
+  </si>
+  <si>
+    <t>fonts.googleapis.com</t>
+  </si>
+  <si>
+    <t>Price Spider</t>
+  </si>
+  <si>
+    <t>cdn.pricespider.com</t>
+  </si>
+  <si>
+    <t>Google Recaptcha</t>
+  </si>
+  <si>
+    <t>Google Classic Analytics</t>
+  </si>
+  <si>
+    <t>Google Botguard</t>
+  </si>
+  <si>
+    <t>www.abreva.ca</t>
+  </si>
+  <si>
+    <t>collect.analyze.ly</t>
+  </si>
+  <si>
+    <t>fonts.gstatic.com</t>
+  </si>
+  <si>
+    <t>www.gsk.com</t>
+  </si>
+  <si>
+    <t>abreva-ca-preview.gdsgsk.com</t>
+  </si>
+  <si>
+    <t>a-cf65ch.gskstatic.com</t>
+  </si>
+  <si>
+    <t>www.google.com.bd</t>
+  </si>
+  <si>
+    <t>i-cf65ch.gskstatic.com</t>
+  </si>
+  <si>
+    <t>https://www.google-analytics.com/collect?v=1&amp;_v=j90&amp;a=1479768383&amp;t=pageview&amp;_s=1&amp;dl=https%3A%2F%2Fwww.advil.com%2F&amp;ul=en-us&amp;de=UTF-8&amp;dt=Advil%20Pain%20Relief%20Medicine%20%7C%20Advil&amp;sd=24-bit&amp;sr=1680x927&amp;vp=1680x927&amp;je=0&amp;_u=YCDAgEAB~&amp;jid=611607466&amp;gjid=1822327957&amp;cid=343336703.1619917887&amp;tid=UA-55526842-1&amp;_gid=669086690.1619917888&amp;gtm=2wg4l3MMH8CL6&amp;z=245748634</t>
+  </si>
+  <si>
+    <t>https://www.google-analytics.com/g/collect?v=2&amp;tid=G-EXM44P7M32&amp;gtm=2oe4l3&amp;_p=1479768383&amp;sr=1680x927&amp;ul=en-us&amp;cid=343336703.1619917887&amp;_s=1&amp;dl=https%3A%2F%2Fwww.advil.com%2F&amp;dt=Advil%20Pain%20Relief%20Medicine%20%7C%20Advil&amp;sid=1619917887&amp;sct=1&amp;seg=0&amp;en=page_view&amp;_fv=1&amp;_nsi=1&amp;_ss=1</t>
+  </si>
+  <si>
+    <t>https://www.google-analytics.com/j/collect?v=1&amp;_v=j90&amp;a=1479768383&amp;t=pageview&amp;_s=1&amp;dl=https%3A%2F%2Fwww.advil.com%2F&amp;ul=en-us&amp;de=UTF-8&amp;dt=Advil%20Pain%20Relief%20Medicine%20%7C%20Advil&amp;sd=24-bit&amp;sr=1680x927&amp;vp=1680x927&amp;je=0&amp;_u=YCDAAEABAAAAAG~&amp;jid=1534424798&amp;gjid=1435325694&amp;cid=343336703.1619917887&amp;tid=UA-135635203-1&amp;_gid=669086690.1619917888&amp;_r=1&amp;gtm=2wg4l3MMH8CL6&amp;z=1920179212</t>
+  </si>
+  <si>
+    <t>https://www.googletagmanager.com/gtm.js?id=GTM-MMH8CL6</t>
   </si>
   <si>
     <t>onetrust.com</t>
   </si>
   <si>
-    <t>youtube.com</t>
-  </si>
-  <si>
-    <t>themes.googleusercontent.com</t>
-  </si>
-  <si>
-    <t>cdn.cookielaw.org</t>
-  </si>
-  <si>
-    <t>cookiepedia.co.uk</t>
-  </si>
-  <si>
-    <t>stats.g.doubleclick.net</t>
-  </si>
-  <si>
-    <t>d22xmn10vbouk4.cloudfront.net</t>
-  </si>
-  <si>
-    <t>www.google.com</t>
-  </si>
-  <si>
-    <t>www.theraflu.com</t>
-  </si>
-  <si>
-    <t>terms.gsk.com</t>
-  </si>
-  <si>
-    <t>www.google.com.bd</t>
-  </si>
-  <si>
-    <t>cookies.gsk.com</t>
-  </si>
-  <si>
-    <t>www.youtube.com</t>
-  </si>
-  <si>
-    <t>where-to-buy.co</t>
-  </si>
-  <si>
-    <t>www.triaminic.com</t>
-  </si>
-  <si>
-    <t>geolocation.onetrust.com</t>
-  </si>
-  <si>
-    <t>Google Web Font</t>
-  </si>
-  <si>
-    <t>fonts.googleapis.com</t>
-  </si>
-  <si>
-    <t>Price Spider</t>
-  </si>
-  <si>
-    <t>cdn.pricespider.com</t>
+    <t>t.co</t>
+  </si>
+  <si>
+    <t>https://9815642.fls.doubleclick.net/activityi;src=9815642;type=advil;cat=advapstd;ord=1247423365076;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://9815642.fls.doubleclick.net/activityi;dc_pre=CMiz5rLoqfACFQbLjwod1uIKQg;src=9815642;type=advil;cat=advapunq;ord=1;num=8529221149710;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://9815642.fls.doubleclick.net/activityi;dc_pre=CNWy5rLoqfACFQ5JjwodYQIHIQ;src=9815642;type=advil;cat=advapstd;ord=1247423365076;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://9811035.fls.doubleclick.net/activityi;src=9811035;type=advilda;cat=adaapunq;ord=1;num=3587092320636;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://9811035.fls.doubleclick.net/activityi;dc_pre=CN2a6LLoqfACFRnfjwoda-UNgg;src=9811035;type=advilda;cat=adaapstd;ord=7881377672950;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://cm.g.doubleclick.net/pixel?google_nid=TheTradeDesk&amp;google_cm&amp;google_sc&amp;google_hm=NjZmZDViMTMtNGY1ZC00ZDFmLTliNjQtMjY2NjQzNDdiMDQ2&amp;gdpr=0&amp;gdpr_consent=&amp;ttd_tdid=66fd5b13-4f5d-4d1f-9b64-26664347b046</t>
+  </si>
+  <si>
+    <t>https://9811035.fls.doubleclick.net/activityi;src=9811035;type=advilda;cat=adaapstd;ord=7881377672950;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://9815642.fls.doubleclick.net/activityi;src=9815642;type=advil;cat=advapunq;ord=1;num=8529221149710;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>https://stats.g.doubleclick.net/j/collect?t=dc&amp;aip=1&amp;_r=3&amp;v=1&amp;_v=j90&amp;tid=UA-55526842-1&amp;cid=343336703.1619917887&amp;jid=611607466&amp;gjid=1822327957&amp;_gid=669086690.1619917888&amp;_u=YCDAgEABAAAAAE~&amp;z=1164146674</t>
+  </si>
+  <si>
+    <t>https://9811035.fls.doubleclick.net/activityi;dc_pre=CMed6LLoqfACFddBnQkdfyMMHg;src=9811035;type=advilda;cat=adaapunq;ord=1;num=3587092320636;gtm=2wg4l3;auiddc=949154555.1619917887;~oref=https%3A%2F%2Fwww.advil.com%2F?</t>
+  </si>
+  <si>
+    <t>doubleclick.net</t>
+  </si>
+  <si>
+    <t>9811035.fls.doubleclick.net</t>
+  </si>
+  <si>
+    <t>cm.g.doubleclick.net</t>
+  </si>
+  <si>
+    <t>9815642.fls.doubleclick.net</t>
+  </si>
+  <si>
+    <t>https://www.googletagmanager.com/gtag/js?id=G-EXM44P7M32&amp;l=dataLayer&amp;cx=c</t>
+  </si>
+  <si>
+    <t>The Trade Desk</t>
+  </si>
+  <si>
+    <t>insight.adsrvr.org</t>
+  </si>
+  <si>
+    <t>adsrvr.org</t>
+  </si>
+  <si>
+    <t>Google Authorized Buyers - Cookie Match</t>
+  </si>
+  <si>
+    <t>Verizon Media</t>
+  </si>
+  <si>
+    <t>yahoo.com</t>
+  </si>
+  <si>
+    <t>analytics.yahoo.com</t>
+  </si>
+  <si>
+    <t>https://ups.analytics.yahoo.com/ups/55953/sync?uid=66fd5b13-4f5d-4d1f-9b64-26664347b046&amp;_origin=1&amp;gdpr=0&amp;gdpr_consent=&amp;verify=true</t>
+  </si>
+  <si>
+    <t>ups.analytics.yahoo.com</t>
+  </si>
+  <si>
+    <t>Facebook Pixel</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tr/?id=436957850274279&amp;ev=Microdata&amp;dl=https%3A%2F%2Fwww.advil.com%2F&amp;rl=&amp;if=false&amp;ts=1619917889238&amp;cd[DataLayer]=%5B%5D&amp;cd[Meta]=%7B%22title%22%3A%22Advil%20Pain%20Relief%20Medicine%20%7C%20Advil%22%2C%22meta%3Akeywords%22%3A%22pain%20relief%2Cpain%20relief%20medicine%22%2C%22meta%3Adescription%22%3A%22Official%20website%20for%20Advil%20(Ibuprofen)%20NSAID%20analgesic%20pain%20relief%20products.%20Advil%20delivers%20relief%20that%26%23039%3Bs%20fast%20with%20strength%20that%20lasts.%22%7D&amp;cd[OpenGraph]=%7B%22og%3Atype%22%3A%22website%22%2C%22og%3Aurl%22%3A%22https%3A%2F%2Fwww.advil.com%2F%22%2C%22og%3Adescription%22%3A%22Official%20website%20for%20Advil%20(Ibuprofen)%20NSAID%20analgesic%20pain%20relief%20products.%20Advil%20delivers%20relief%20that%26%23039%3Bs%20fast%20with%20strength%20that%20lasts.%22%2C%22og%3Atitle%22%3A%22Homepage%20(US)%22%7D&amp;cd[Schema.org]=%5B%5D&amp;cd[JSON-LD]=%5B%7B%22%40context%22%3A%22https%3A%2F%2Fschema.org%2F%22%2C%22%40type%22%3A%22WebSite%22%2C%22name%22%3A%22Advil%22%2C%22url%22%3A%22https%3A%2F%2Fwww.advil.com%2F%22%2C%22potentialAction%22%3A%7B%22%40type%22%3A%22SearchAction%22%2C%22target%22%3A%22https%3A%2F%2Fwww.advil.com%2Fsite-search%2F%3F_charset_%3DUTF-8%26q%3D%7Bsearch_term_string%7D%22%2C%22query-input%22%3A%22required%20name%3Dsearch_term_string%22%7D%7D%5D&amp;sw=1680&amp;sh=927&amp;v=2.9.39&amp;r=stable&amp;ec=1&amp;o=30&amp;fbp=fb.1.1619917888704.2098550927&amp;it=1619917887953&amp;coo=false&amp;es=automatic&amp;tm=3&amp;exp=l1&amp;rqm=GET</t>
+  </si>
+  <si>
+    <t>www.facebook.com</t>
+  </si>
+  <si>
+    <t>facebook.com</t>
+  </si>
+  <si>
+    <t>Gigya</t>
+  </si>
+  <si>
+    <t>gigya.com</t>
+  </si>
+  <si>
+    <t>cdns.gigya.com</t>
+  </si>
+  <si>
+    <t>cdns.us1.gigya.com</t>
+  </si>
+  <si>
+    <t>accounts.us1.gigya.com</t>
+  </si>
+  <si>
+    <t>Google Optimize</t>
+  </si>
+  <si>
+    <t>www.googleoptimize.com</t>
+  </si>
+  <si>
+    <t>Rubicon Project</t>
+  </si>
+  <si>
+    <t>rubiconproject.com</t>
+  </si>
+  <si>
+    <t>Facebook Social Plugins</t>
+  </si>
+  <si>
+    <t>https://connect.facebook.net/en_US/fbevents.js</t>
+  </si>
+  <si>
+    <t>https://connect.facebook.net/signals/config/436957850274279?v=2.9.39&amp;r=stable</t>
+  </si>
+  <si>
+    <t>connect.facebook.net</t>
+  </si>
+  <si>
+    <t>Google Ads Remarketing</t>
+  </si>
+  <si>
+    <t>MediaMath</t>
+  </si>
+  <si>
+    <t>https://pixel.mathtag.com/misc/img?mm_bnc&amp;bcdv=0</t>
+  </si>
+  <si>
+    <t>https://pixel.mathtag.com/sync/js?sync=auto&amp;exsync=https%3A%2F%2Fc212.net%2Fc%2Fsync%3Fu%3D%26c%3DUS%26dmpId%3D1%26pid%3D%5BMM_UUID%5D&amp;mt_lim=1</t>
+  </si>
+  <si>
+    <t>pixel.mathtag.com</t>
+  </si>
+  <si>
+    <t>mathtag.com</t>
+  </si>
+  <si>
+    <t>Twitter Widget</t>
+  </si>
+  <si>
+    <t>twitter.com</t>
+  </si>
+  <si>
+    <t>Twitter Conversion Tracking</t>
+  </si>
+  <si>
+    <t>advil.fr</t>
+  </si>
+  <si>
+    <t>pixel.rubiconproject.com</t>
+  </si>
+  <si>
+    <t>www.advil.com.mx</t>
+  </si>
+  <si>
+    <t>www.advil.hu</t>
+  </si>
+  <si>
+    <t>respiratory.advil.com</t>
+  </si>
+  <si>
+    <t>www.advil.com.co</t>
+  </si>
+  <si>
+    <t>www.advil.com</t>
+  </si>
+  <si>
+    <t>pm.advil.com</t>
+  </si>
+  <si>
+    <t>www.advil.com.br</t>
+  </si>
+  <si>
+    <t>us.gsk.com</t>
+  </si>
+  <si>
+    <t>www.advil.co.nz</t>
+  </si>
+  <si>
+    <t>www.advilpr.com</t>
+  </si>
+  <si>
+    <t>adservice.google.com</t>
+  </si>
+  <si>
+    <t>cdn.c212.net</t>
+  </si>
+  <si>
+    <t>www.advil.net.au</t>
+  </si>
+  <si>
+    <t>c212.net</t>
+  </si>
+  <si>
+    <t>childrens.advil.com</t>
+  </si>
+  <si>
+    <t>www.advil.nl</t>
+  </si>
+  <si>
+    <t>www.advil.ca</t>
+  </si>
+  <si>
+    <t>js.adsrvr.org</t>
+  </si>
+  <si>
+    <t>adservice.google.com.bd</t>
+  </si>
+  <si>
+    <t>match.adsrvr.org</t>
+  </si>
+  <si>
+    <t>www.advilkorea.com</t>
+  </si>
+  <si>
+    <t>www.gskhealthpartner.com</t>
+  </si>
+  <si>
+    <t>www.instagram.com</t>
+  </si>
+  <si>
+    <t>https://www.googletagmanager.com/gtm.js?id=GTM-P9W85WW</t>
+  </si>
+  <si>
+    <t>Fonts.com</t>
+  </si>
+  <si>
+    <t>fast.fonts.net</t>
+  </si>
+  <si>
+    <t>Cloud.typography</t>
+  </si>
+  <si>
+    <t>cloud.typography.com</t>
   </si>
   <si>
     <t>i-cf5.gskstatic.com</t>
   </si>
   <si>
-    <t>fonts.gstatic.com</t>
-  </si>
-  <si>
-    <t>www.abreva.ca</t>
-  </si>
-  <si>
-    <t>abreva-ca-preview.gdsgsk.com</t>
-  </si>
-  <si>
-    <t>a-cf5.gskstatic.com</t>
-  </si>
-  <si>
-    <t>www.gsk.com</t>
-  </si>
-  <si>
-    <t>DoubleClick</t>
-  </si>
-  <si>
-    <t>doubleclick.net</t>
-  </si>
-  <si>
-    <t>Google Authorized Buyers - Cookie Match</t>
-  </si>
-  <si>
-    <t>cm.g.doubleclick.net</t>
-  </si>
-  <si>
-    <t>Verizon Media</t>
-  </si>
-  <si>
-    <t>yahoo.com</t>
-  </si>
-  <si>
-    <t>analytics.yahoo.com</t>
-  </si>
-  <si>
-    <t>ups.analytics.yahoo.com</t>
-  </si>
-  <si>
-    <t>Gigya</t>
-  </si>
-  <si>
-    <t>cdns.gigya.com</t>
-  </si>
-  <si>
-    <t>gigya.com</t>
-  </si>
-  <si>
-    <t>cdns.us1.gigya.com</t>
-  </si>
-  <si>
-    <t>accounts.us1.gigya.com</t>
-  </si>
-  <si>
-    <t>Rubicon Project</t>
-  </si>
-  <si>
-    <t>rubiconproject.com</t>
-  </si>
-  <si>
-    <t>t.co</t>
-  </si>
-  <si>
-    <t>Facebook Social Plugins</t>
-  </si>
-  <si>
-    <t>connect.facebook.net</t>
-  </si>
-  <si>
-    <t>Twitter Conversion Tracking</t>
-  </si>
-  <si>
-    <t>twitter.com</t>
-  </si>
-  <si>
-    <t>pixel.mathtag.com</t>
-  </si>
-  <si>
-    <t>www.instagram.com</t>
-  </si>
-  <si>
-    <t>9815642.fls.doubleclick.net</t>
-  </si>
-  <si>
-    <t>www.gskhealthpartner.com</t>
-  </si>
-  <si>
-    <t>9811035.fls.doubleclick.net</t>
-  </si>
-  <si>
-    <t>cdn.c212.net</t>
-  </si>
-  <si>
-    <t>childrens.advil.com</t>
-  </si>
-  <si>
-    <t>adservice.google.com.bd</t>
-  </si>
-  <si>
-    <t>adsrvr.org</t>
-  </si>
-  <si>
-    <t>www.advil.ca</t>
-  </si>
-  <si>
-    <t>www.advilpr.com</t>
-  </si>
-  <si>
-    <t>www.advil.com.co</t>
-  </si>
-  <si>
-    <t>www.advil.net.au</t>
-  </si>
-  <si>
-    <t>www.facebook.com</t>
-  </si>
-  <si>
-    <t>www.advil.com.mx</t>
-  </si>
-  <si>
-    <t>www.advil.hu</t>
-  </si>
-  <si>
-    <t>js.adsrvr.org</t>
-  </si>
-  <si>
-    <t>www.advilkorea.com</t>
-  </si>
-  <si>
-    <t>pm.advil.com</t>
-  </si>
-  <si>
-    <t>match.adsrvr.org</t>
-  </si>
-  <si>
-    <t>c212.net</t>
-  </si>
-  <si>
-    <t>facebook.com</t>
-  </si>
-  <si>
-    <t>www.advil.com</t>
-  </si>
-  <si>
-    <t>insight.adsrvr.org</t>
-  </si>
-  <si>
-    <t>us.gsk.com</t>
-  </si>
-  <si>
-    <t>pixel.rubiconproject.com</t>
-  </si>
-  <si>
-    <t>mathtag.com</t>
-  </si>
-  <si>
-    <t>adservice.google.com</t>
-  </si>
-  <si>
-    <t>www.advil.co.nz</t>
-  </si>
-  <si>
-    <t>respiratory.advil.com</t>
-  </si>
-  <si>
-    <t>www.googleoptimize.com</t>
-  </si>
-  <si>
-    <t>www.advil.nl</t>
-  </si>
-  <si>
-    <t>www.advil.com.br</t>
-  </si>
-  <si>
-    <t>advil.fr</t>
-  </si>
-  <si>
-    <t>Cloud.typography</t>
-  </si>
-  <si>
-    <t>cloud.typography.com</t>
-  </si>
-  <si>
-    <t>fast.fonts.net</t>
+    <t>www.aquafresh.bg</t>
   </si>
   <si>
     <t>bg.gsk.com</t>
-  </si>
-  <si>
-    <t>collect.analyze.ly</t>
-  </si>
-  <si>
-    <t>www.aquafresh.bg</t>
   </si>
 </sst>
 </file>
@@ -752,18 +876,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B22" sqref="B22"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,10 +916,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,16 +927,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -822,6 +948,9 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -830,16 +959,22 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,26 +1059,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +1098,7 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,10 +1106,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
         <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,10 +1117,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,10 +1128,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -995,82 +1139,109 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,95 +1289,71 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,10 +1361,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1372,10 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,10 +1383,10 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,10 +1394,10 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,10 +1405,10 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,10 +1427,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1438,10 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,10 +1449,10 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,10 +1460,10 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,10 +1471,10 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,10 +1482,10 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,10 +1493,10 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1357,10 +1504,10 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C64" t="s">
         <v>60</v>
@@ -1378,564 +1525,1172 @@
       <c r="A65" t="s">
         <v>3</v>
       </c>
+      <c r="B65" t="s">
+        <v>35</v>
+      </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>3</v>
       </c>
+      <c r="B66" t="s">
+        <v>35</v>
+      </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>3</v>
       </c>
+      <c r="B68" t="s">
+        <v>35</v>
+      </c>
       <c r="C68" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
       <c r="C69" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
+      <c r="B70" t="s">
+        <v>35</v>
+      </c>
       <c r="C70" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>3</v>
       </c>
+      <c r="B71" t="s">
+        <v>35</v>
+      </c>
       <c r="C71" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>3</v>
       </c>
+      <c r="B72" t="s">
+        <v>35</v>
+      </c>
       <c r="C72" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
+      <c r="B73" t="s">
+        <v>35</v>
+      </c>
       <c r="C73" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
+      <c r="B74" t="s">
+        <v>35</v>
+      </c>
       <c r="C74" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>3</v>
       </c>
+      <c r="B75" t="s">
+        <v>35</v>
+      </c>
       <c r="C75" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
+      <c r="B76" t="s">
+        <v>35</v>
+      </c>
       <c r="C76" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>3</v>
       </c>
+      <c r="B77" t="s">
+        <v>35</v>
+      </c>
       <c r="C77" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>3</v>
       </c>
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
       <c r="C78" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
+      <c r="B79" t="s">
+        <v>16</v>
+      </c>
       <c r="C79" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>3</v>
       </c>
+      <c r="B80" t="s">
+        <v>16</v>
+      </c>
       <c r="C80" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>3</v>
       </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
       <c r="C81" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>3</v>
       </c>
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
       <c r="C82" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>3</v>
       </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>3</v>
       </c>
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>3</v>
       </c>
+      <c r="B85" t="s">
+        <v>77</v>
+      </c>
       <c r="C85" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>3</v>
       </c>
+      <c r="B86" t="s">
+        <v>78</v>
+      </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>3</v>
       </c>
+      <c r="B87" t="s">
+        <v>78</v>
+      </c>
       <c r="C87" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
+      <c r="B88" t="s">
+        <v>78</v>
+      </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>3</v>
       </c>
+      <c r="B89" t="s">
+        <v>78</v>
+      </c>
       <c r="C89" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>3</v>
       </c>
+      <c r="B90" t="s">
+        <v>78</v>
+      </c>
       <c r="C90" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>3</v>
       </c>
+      <c r="B91" t="s">
+        <v>78</v>
+      </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>3</v>
       </c>
+      <c r="B92" t="s">
+        <v>78</v>
+      </c>
       <c r="C92" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>3</v>
       </c>
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
       <c r="C93" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>3</v>
       </c>
+      <c r="B94" t="s">
+        <v>83</v>
+      </c>
       <c r="C94" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>3</v>
       </c>
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
       <c r="C95" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>3</v>
       </c>
+      <c r="B96" t="s">
+        <v>87</v>
+      </c>
       <c r="C96" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
+      <c r="B97" t="s">
+        <v>87</v>
+      </c>
       <c r="C97" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>3</v>
       </c>
+      <c r="B98" t="s">
+        <v>87</v>
+      </c>
       <c r="C98" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>3</v>
       </c>
+      <c r="B99" t="s">
+        <v>87</v>
+      </c>
       <c r="C99" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>3</v>
       </c>
+      <c r="B100" t="s">
+        <v>87</v>
+      </c>
       <c r="C100" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>3</v>
       </c>
+      <c r="B101" t="s">
+        <v>87</v>
+      </c>
       <c r="C101" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
+      <c r="B102" t="s">
+        <v>92</v>
+      </c>
       <c r="C102" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>3</v>
       </c>
+      <c r="B103" t="s">
+        <v>94</v>
+      </c>
       <c r="C103" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>3</v>
       </c>
+      <c r="B104" t="s">
+        <v>94</v>
+      </c>
       <c r="C104" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>3</v>
       </c>
+      <c r="B105" t="s">
+        <v>96</v>
+      </c>
       <c r="C105" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
+      <c r="B106" t="s">
+        <v>96</v>
+      </c>
       <c r="C106" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>3</v>
       </c>
+      <c r="B107" t="s">
+        <v>96</v>
+      </c>
       <c r="C107" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>3</v>
       </c>
+      <c r="B108" t="s">
+        <v>100</v>
+      </c>
       <c r="C108" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>3</v>
       </c>
+      <c r="B109" t="s">
+        <v>101</v>
+      </c>
       <c r="C109" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>3</v>
       </c>
+      <c r="B110" t="s">
+        <v>101</v>
+      </c>
       <c r="C110" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>3</v>
       </c>
+      <c r="B111" t="s">
+        <v>101</v>
+      </c>
       <c r="C111" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>3</v>
       </c>
+      <c r="B112" t="s">
+        <v>101</v>
+      </c>
       <c r="C112" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>3</v>
       </c>
+      <c r="B113" t="s">
+        <v>17</v>
+      </c>
       <c r="C113" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B114" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" t="s">
         <v>11</v>
-      </c>
-      <c r="C114" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="C115" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C116" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>43</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B119" t="s">
+        <v>43</v>
       </c>
       <c r="C119" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B120" t="s">
+        <v>43</v>
       </c>
       <c r="C120" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B121" t="s">
+        <v>43</v>
       </c>
       <c r="C121" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>43</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B123" t="s">
+        <v>44</v>
       </c>
       <c r="C123" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C125" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C127" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C129" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C130" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C131" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C132" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>3</v>
+      </c>
+      <c r="C138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="C146" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>5</v>
       </c>
-      <c r="C133" t="s">
-        <v>30</v>
+      <c r="B160" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" t="s">
+        <v>38</v>
+      </c>
+      <c r="C166" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" t="s">
+        <v>16</v>
+      </c>
+      <c r="C167" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" t="s">
+        <v>135</v>
+      </c>
+      <c r="C168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" t="s">
+        <v>137</v>
+      </c>
+      <c r="C169" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>17</v>
+      </c>
+      <c r="C170" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>5</v>
+      </c>
+      <c r="C171" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>5</v>
+      </c>
+      <c r="C177" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>5</v>
+      </c>
+      <c r="C178" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>5</v>
+      </c>
+      <c r="C181" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>